<commit_message>
Inclusion of Common IC Type information in 2010 data
</commit_message>
<xml_diff>
--- a/DataOverview/W4CW-BQE-overview.xlsx
+++ b/DataOverview/W4CW-BQE-overview.xlsx
@@ -998,7 +998,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>

</xml_diff>